<commit_message>
09.08 Signed-off-by: sytt3 <782528429@qq.com>
</commit_message>
<xml_diff>
--- a/科大讯飞营销大赛数据集/字段解释.xlsx
+++ b/科大讯飞营销大赛数据集/字段解释.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git-Item\item\科大讯飞营销大赛数据集\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFDF2D8-E3AD-411B-86DD-2CAF119921C0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871E0DE4-0D99-40BF-82A2-F661D135D17D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="83">
   <si>
     <t>字段名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -332,12 +332,16 @@
     <t>画图探究</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>09.08进度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -350,6 +354,13 @@
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -379,11 +390,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -396,7 +408,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -677,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -692,7 +705,7 @@
     <col min="6" max="6" width="31.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -708,8 +721,11 @@
       <c r="E1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -729,7 +745,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -745,11 +761,15 @@
       <c r="E3" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="7">
+        <v>1</v>
+      </c>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -765,11 +785,15 @@
       <c r="E4" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="7">
+        <v>1</v>
+      </c>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -785,8 +809,10 @@
       <c r="E5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -802,11 +828,12 @@
       <c r="E6" t="s">
         <v>76</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -823,7 +850,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -839,11 +866,14 @@
       <c r="E8" t="s">
         <v>76</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -859,11 +889,12 @@
       <c r="E9" t="s">
         <v>76</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -880,7 +911,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -897,7 +928,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -913,11 +944,12 @@
       <c r="E12" t="s">
         <v>76</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -934,7 +966,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -950,11 +982,12 @@
       <c r="E14" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -970,11 +1003,12 @@
       <c r="E15" t="s">
         <v>76</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -991,7 +1025,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1007,11 +1041,12 @@
       <c r="E17" t="s">
         <v>76</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1028,7 +1063,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -1045,7 +1080,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1062,7 +1097,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1079,7 +1114,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1096,7 +1131,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1113,7 +1148,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -1130,7 +1165,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1147,7 +1182,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -1164,7 +1199,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -1181,7 +1216,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -1201,7 +1236,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -1221,7 +1256,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -1241,7 +1276,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -1261,7 +1296,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -1333,24 +1368,24 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
     </row>
     <row r="38" spans="1:6" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>

</xml_diff>